<commit_message>
MML-23: Update GPD comparison. Start analyzing factibility of GDP comparison
</commit_message>
<xml_diff>
--- a/notebooks/data/output/diff_porcentual_DEVELOPED.xlsx
+++ b/notebooks/data/output/diff_porcentual_DEVELOPED.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>POP</t>
+          <t>EXLIFE</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>EXLIFE</t>
+          <t>POP</t>
         </is>
       </c>
     </row>
@@ -455,274 +455,340 @@
         <v>1970</v>
       </c>
       <c r="B2" t="n">
+        <v>2.077964146380993</v>
+      </c>
+      <c r="C2" t="n">
         <v>-2.003545998855764</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2.077964146380993</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="B3" t="n">
-        <v>-2.589179606070642</v>
+        <v>1.629676583197283</v>
       </c>
       <c r="C3" t="n">
-        <v>1.451025082649725</v>
+        <v>-2.297414531294307</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="B4" t="n">
-        <v>-3.128794008214898</v>
+        <v>1.451025082649725</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9595423333267967</v>
+        <v>-2.589179606070642</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1976</v>
+        <v>1973</v>
       </c>
       <c r="B5" t="n">
-        <v>-3.642458742718181</v>
+        <v>1.319655521783184</v>
       </c>
       <c r="C5" t="n">
-        <v>1.512510542592103</v>
+        <v>-2.870203871394999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1978</v>
+        <v>1974</v>
       </c>
       <c r="B6" t="n">
-        <v>-4.045831393300558</v>
+        <v>0.9595423333267967</v>
       </c>
       <c r="C6" t="n">
-        <v>0.587631647009409</v>
+        <v>-3.128794008214898</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1980</v>
+        <v>1975</v>
       </c>
       <c r="B7" t="n">
-        <v>-4.383012834506642</v>
+        <v>1.047385877238197</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2717797421690484</v>
+        <v>-3.447302315816906</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1982</v>
+        <v>1976</v>
       </c>
       <c r="B8" t="n">
-        <v>-4.673415949706177</v>
+        <v>1.512510542592103</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0576303714815217</v>
+        <v>-3.642458742718181</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1984</v>
+        <v>1977</v>
       </c>
       <c r="B9" t="n">
-        <v>-5.024024836728129</v>
+        <v>0.7960237858824354</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.6374861549821504</v>
+        <v>-3.90015600624025</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1986</v>
+        <v>1978</v>
       </c>
       <c r="B10" t="n">
-        <v>-5.300563575084385</v>
+        <v>0.587631647009409</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.28264279782225</v>
+        <v>-4.045831393300558</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1988</v>
+        <v>1979</v>
       </c>
       <c r="B11" t="n">
-        <v>-5.579990259306553</v>
+        <v>0.4512004262261842</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.8535509243624568</v>
+        <v>-4.264325406349148</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1990</v>
+        <v>1980</v>
       </c>
       <c r="B12" t="n">
-        <v>-5.774953851048982</v>
+        <v>0.2717797421690484</v>
       </c>
       <c r="C12" t="n">
-        <v>-1.724668094449445</v>
+        <v>-4.383012834506642</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1992</v>
+        <v>1981</v>
       </c>
       <c r="B13" t="n">
-        <v>-5.761916125670259</v>
+        <v>0.05767903960260172</v>
       </c>
       <c r="C13" t="n">
-        <v>-1.50912500472868</v>
+        <v>-4.577586663069531</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1994</v>
+        <v>1982</v>
       </c>
       <c r="B14" t="n">
-        <v>-5.636091580454685</v>
+        <v>0.0576303714815217</v>
       </c>
       <c r="C14" t="n">
-        <v>-1.358501590599233</v>
+        <v>-4.673415949706177</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1996</v>
+        <v>1983</v>
       </c>
       <c r="B15" t="n">
-        <v>-5.254503803389126</v>
+        <v>-0.5347637533183123</v>
       </c>
       <c r="C15" t="n">
-        <v>-2.043200790743082</v>
+        <v>-4.849180384029051</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1998</v>
+        <v>1984</v>
       </c>
       <c r="B16" t="n">
-        <v>-4.800028536211263</v>
+        <v>-0.6374861549821504</v>
       </c>
       <c r="C16" t="n">
-        <v>-2.769759724943003</v>
+        <v>-5.024024836728129</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2000</v>
+        <v>1985</v>
       </c>
       <c r="B17" t="n">
-        <v>-4.267496768240743</v>
+        <v>-0.806042315857238</v>
       </c>
       <c r="C17" t="n">
-        <v>-3.361627094232571</v>
+        <v>-5.117081462313215</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2002</v>
+        <v>1986</v>
       </c>
       <c r="B18" t="n">
-        <v>-4.640267132313975</v>
+        <v>-1.28264279782225</v>
       </c>
       <c r="C18" t="n">
-        <v>-3.085111703681882</v>
+        <v>-5.300563575084385</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2004</v>
+        <v>1987</v>
       </c>
       <c r="B19" t="n">
-        <v>-5.068077201990158</v>
+        <v>-1.164401421074917</v>
       </c>
       <c r="C19" t="n">
-        <v>-3.666577703816509</v>
+        <v>-5.402573417371694</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2006</v>
+        <v>1988</v>
       </c>
       <c r="B20" t="n">
-        <v>-5.50420694655567</v>
+        <v>-0.8535509243624568</v>
       </c>
       <c r="C20" t="n">
-        <v>-4.237371898246902</v>
+        <v>-5.579990259306553</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2008</v>
+        <v>1989</v>
       </c>
       <c r="B21" t="n">
-        <v>-6.166291306443984</v>
+        <v>-1.707078776625043</v>
       </c>
       <c r="C21" t="n">
-        <v>-4.940072604840648</v>
+        <v>-5.734913050147707</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2010</v>
+        <v>1990</v>
       </c>
       <c r="B22" t="n">
-        <v>-6.799346161566919</v>
+        <v>-1.724668094449445</v>
       </c>
       <c r="C22" t="n">
-        <v>-5.740531655875338</v>
+        <v>-5.774953851048982</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2012</v>
+        <v>1991</v>
       </c>
       <c r="B23" t="n">
-        <v>-7.342403499134048</v>
+        <v>-1.69291274863643</v>
       </c>
       <c r="C23" t="n">
-        <v>-6.435692629856206</v>
+        <v>-5.783352285426683</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2014</v>
+        <v>1992</v>
       </c>
       <c r="B24" t="n">
-        <v>-7.96397595623869</v>
+        <v>-1.50912500472868</v>
       </c>
       <c r="C24" t="n">
-        <v>-7.01511573577139</v>
+        <v>-5.761916125670259</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2016</v>
+        <v>1993</v>
       </c>
       <c r="B25" t="n">
-        <v>-8.548030353203732</v>
+        <v>-1.398436866160009</v>
       </c>
       <c r="C25" t="n">
-        <v>-7.302611204689141</v>
+        <v>-5.712436666954835</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2018</v>
+        <v>1994</v>
       </c>
       <c r="B26" t="n">
-        <v>-9.090176537940017</v>
+        <v>-1.358501590599233</v>
       </c>
       <c r="C26" t="n">
-        <v>-7.660184945988443</v>
+        <v>-5.636091580454685</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1995</v>
+      </c>
+      <c r="B27" t="n">
+        <v>-1.475300003782098</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-5.456293566220656</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1996</v>
+      </c>
+      <c r="B28" t="n">
+        <v>-2.043200790743082</v>
+      </c>
+      <c r="C28" t="n">
+        <v>-5.254503803389126</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1997</v>
+      </c>
+      <c r="B29" t="n">
+        <v>-2.495669468146511</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-5.032785164116709</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>1998</v>
+      </c>
+      <c r="B30" t="n">
+        <v>-2.769759724943003</v>
+      </c>
+      <c r="C30" t="n">
+        <v>-4.800028536211263</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>1999</v>
+      </c>
+      <c r="B31" t="n">
+        <v>-3.015024624650196</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-4.568468568819327</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B32" t="n">
+        <v>-3.361627094232571</v>
+      </c>
+      <c r="C32" t="n">
+        <v>-4.267496768240743</v>
       </c>
     </row>
   </sheetData>

</xml_diff>